<commit_message>
uploading risk analysis checked and fixed
</commit_message>
<xml_diff>
--- a/docs/360 Müşteri Riski Analiz Sistemi new.xlsx
+++ b/docs/360 Müşteri Riski Analiz Sistemi new.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Ana Sayfa" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="316">
   <si>
     <t>Yazılım Logo</t>
   </si>
@@ -722,12 +722,6 @@
     <t>(Müşteri Adı, Limit, Teminat Durumu, İl)</t>
   </si>
   <si>
-    <t xml:space="preserve">Uyarılar, zaman damgalı düşecek, popup şeklinde bilidirm açılacak, bildiirimden tıklandığında veya dashboarddan tıklandığında aksyion </t>
-  </si>
-  <si>
-    <t>menüsü gelecek. Menüde kullanıcı aksiyon tanımlayacak ve kaydete bastığında bu aksiyonu yazdıracağız.</t>
-  </si>
-  <si>
     <t>Çek uyarı</t>
   </si>
   <si>
@@ -996,6 +990,21 @@
   </si>
   <si>
     <t>SAP'te varsa alırız (II. Faz)</t>
+  </si>
+  <si>
+    <t>Şimdi koymadım</t>
+  </si>
+  <si>
+    <t>Uyarılar, zaman damgalı düşecek, popup şeklinde bildirim açılacak, bildirimden tıklandığında veya dashboarddan tıklandığında aksyion menüsü gelecek. Menüde kullanıcı aksiyon tanımlayacak ve kaydete bastığında bu aksiyonu yazdıracağız.</t>
+  </si>
+  <si>
+    <t>Aralık? Ne aralığı? Nerede veriyoruz?</t>
+  </si>
+  <si>
+    <t>Nerede alıyoruz bu veriyi?</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1092,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1124,6 +1133,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1308,44 +1323,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1412,9 +1391,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1473,6 +1449,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1923,481 +1939,481 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.05" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="64"/>
+      <c r="C2" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
       <c r="M2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
       <c r="M3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="10" t="s">
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="16"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="4"/>
       <c r="M5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="17" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="16"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="16"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="16"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="16"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="16"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="16"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="16"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="16"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="10" t="s">
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="16"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="17" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="16"/>
+      <c r="L16" s="4"/>
     </row>
     <row r="17" spans="3:12">
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="16"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="4"/>
     </row>
     <row r="18" spans="3:12">
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="16"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="4"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="16"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="3:12">
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="16"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="3:12">
-      <c r="C21" s="26"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="16"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="3:12">
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="16"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="3:12">
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="31"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="19"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="3:12">
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="34"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="26" spans="3:12">
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="10" t="s">
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="16"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" spans="3:12">
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="17" t="s">
+      <c r="G27" s="3"/>
+      <c r="H27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="J27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="19" t="s">
+      <c r="K27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L27" s="16"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="3:12">
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="16"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" spans="3:12">
-      <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="16"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" spans="3:12">
-      <c r="C30" s="20"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="16"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="4"/>
     </row>
     <row r="31" spans="3:12">
-      <c r="C31" s="20"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="16"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="3:12">
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="16"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="4"/>
     </row>
     <row r="33" spans="2:12">
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="16"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="4"/>
     </row>
     <row r="34" spans="2:12">
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="31"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="19"/>
     </row>
     <row r="35" spans="2:12">
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="34"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="22"/>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="35">
+      <c r="B40" s="23">
         <v>1</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="24" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2440,13 +2456,13 @@
       <c r="C45" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="37"/>
+      <c r="F45" s="25"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="35">
+      <c r="B47" s="23">
         <v>2</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="24" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2476,10 +2492,10 @@
       </c>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="35">
+      <c r="B54" s="23">
         <v>3</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2526,24 +2542,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.19921875" style="38" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" style="26" customWidth="1"/>
     <col min="2" max="2" width="51.296875" customWidth="1"/>
     <col min="3" max="4" width="43.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2558,196 +2574,199 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="18" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="31.2">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="27"/>
     </row>
     <row r="10" spans="2:3" ht="31.2">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="39"/>
+      <c r="C10" s="27"/>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="39"/>
+      <c r="C11" s="27"/>
     </row>
     <row r="12" spans="2:3">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="39"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="39"/>
+      <c r="C13" s="27"/>
     </row>
     <row r="14" spans="2:3">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="27"/>
     </row>
     <row r="15" spans="2:3">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="B17" s="39" t="s">
+    <row r="17" spans="1:4">
+      <c r="B17" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="B18" s="39" t="s">
+    <row r="18" spans="1:4">
+      <c r="B18" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="39" t="s">
+    <row r="19" spans="1:4">
+      <c r="B19" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="39"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="39" t="s">
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="39"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="39" t="s">
+      <c r="C20" s="27"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="39"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" s="39" t="s">
+      <c r="C21" s="27"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="39"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="41"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="41">
+      <c r="C22" s="27"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="29"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="29">
         <v>1</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="41"/>
-      <c r="B25" s="42" t="s">
+      <c r="C24" s="66"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="29"/>
+      <c r="B25" s="30" t="s">
         <v>66</v>
       </c>
       <c r="C25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="29"/>
+      <c r="B26" s="30" t="s">
         <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="29"/>
+      <c r="B27" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="41">
+    <row r="28" spans="1:4">
+      <c r="A28" s="29">
         <v>2</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="41"/>
-      <c r="B29" s="42" t="s">
+      <c r="C28" s="66"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="29"/>
+      <c r="B29" s="30" t="s">
         <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" s="29"/>
+      <c r="B30" s="30" t="s">
         <v>72</v>
       </c>
       <c r="C30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="41">
+    <row r="31" spans="1:4">
+      <c r="A31" s="29">
         <v>3</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="76" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="41"/>
+      <c r="D31" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="29"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="41"/>
+      <c r="A33" s="29"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="41"/>
-      <c r="B34" s="44" t="s">
+      <c r="A34" s="29"/>
+      <c r="B34" s="31" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2757,12 +2776,12 @@
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="41">
+      <c r="A39" s="29">
         <v>1</v>
       </c>
       <c r="B39" t="s">
@@ -2770,7 +2789,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="41">
+      <c r="A40" s="29">
         <v>2</v>
       </c>
       <c r="B40" t="s">
@@ -2778,7 +2797,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="41">
+      <c r="A41" s="29">
         <v>3</v>
       </c>
       <c r="B41" t="s">
@@ -2786,7 +2805,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="41">
+      <c r="A42" s="29">
         <v>4</v>
       </c>
       <c r="B42" t="s">
@@ -2794,7 +2813,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="41">
+      <c r="A43" s="29">
         <v>5</v>
       </c>
       <c r="B43" t="s">
@@ -2802,24 +2821,24 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="41">
+      <c r="A44" s="29">
         <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="41"/>
+      <c r="A45" s="29"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="41"/>
+      <c r="A46" s="29"/>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="41"/>
-      <c r="B47" s="36" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="41">
+      <c r="A48" s="29">
         <v>1</v>
       </c>
       <c r="B48" t="s">
@@ -2827,7 +2846,7 @@
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="41">
+      <c r="A49" s="29">
         <v>2</v>
       </c>
     </row>
@@ -2851,13 +2870,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="5.69921875" style="36" customWidth="1"/>
+    <col min="1" max="1" width="5.69921875" style="24" customWidth="1"/>
     <col min="2" max="2" width="44.19921875" customWidth="1"/>
     <col min="3" max="6" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="41"/>
+      <c r="A1" s="29"/>
       <c r="B1" t="s">
         <v>41</v>
       </c>
@@ -2866,496 +2885,496 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="41"/>
+      <c r="A2" s="29"/>
       <c r="B2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="41"/>
+      <c r="A3" s="29"/>
       <c r="B3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="41"/>
+      <c r="A4" s="29"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="41"/>
+      <c r="A5" s="29"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="41"/>
-      <c r="D6" s="45" t="s">
+      <c r="A6" s="29"/>
+      <c r="D6" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="32" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="46"/>
-      <c r="B8" s="36" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="46">
+      <c r="A9" s="33">
         <v>1</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="46">
+      <c r="A10" s="33">
         <v>2</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="46">
+      <c r="A11" s="33">
         <v>3</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="46">
+      <c r="A12" s="33">
         <v>4</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="46">
+      <c r="A13" s="33">
         <v>8</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="34" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="46">
+      <c r="A14" s="33">
         <v>6</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="46">
+      <c r="A15" s="33">
         <v>7</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="46">
+      <c r="A16" s="33">
         <v>9</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="34" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="46">
+      <c r="A17" s="33">
         <v>10</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="46">
+      <c r="A18" s="33">
         <v>11</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="34" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="46">
+      <c r="A19" s="33">
         <v>12</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="47"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="46">
+      <c r="A20" s="33">
         <v>13</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="47"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="46">
+      <c r="A21" s="33">
         <v>14</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="F21" s="47"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="46">
+      <c r="A22" s="33">
         <v>15</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="46">
+      <c r="A23" s="33">
         <v>16</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="46">
+      <c r="A24" s="33">
         <v>17</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="34" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="46"/>
-      <c r="B31" s="36" t="s">
+      <c r="A31" s="33"/>
+      <c r="B31" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="46">
+      <c r="A32" s="33">
         <v>1</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="46">
+      <c r="A33" s="33">
         <v>2</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="46">
+      <c r="A34" s="33">
         <v>3</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="46">
+      <c r="A35" s="33">
         <v>4</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="46">
+      <c r="A36" s="33">
         <v>5</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="46"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="46"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="46"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="46"/>
-      <c r="B40" s="36" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="46">
+      <c r="A41" s="33">
         <v>1</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="46">
+      <c r="A42" s="33">
         <v>2</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="47" t="s">
+      <c r="C42" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="46">
+      <c r="A43" s="33">
         <v>3</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="46">
+      <c r="A44" s="33">
         <v>4</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3373,7 +3392,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="4.296875" style="46" customWidth="1"/>
+    <col min="1" max="1" width="4.296875" style="33" customWidth="1"/>
     <col min="2" max="2" width="36.69921875" customWidth="1"/>
     <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="5" max="5" width="44.19921875" customWidth="1"/>
@@ -3399,17 +3418,17 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="35" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="32" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3434,215 +3453,215 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8" t="s">
+      <c r="C15" s="69"/>
+      <c r="E15" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="69"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="E16" s="51" t="s">
+      <c r="C16" s="37"/>
+      <c r="E16" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="50"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="E17" s="51" t="s">
+      <c r="C17" s="37"/>
+      <c r="E17" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="50"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="E18" s="51" t="s">
+      <c r="C18" s="37"/>
+      <c r="E18" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="50"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="2:6" ht="31.2">
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="E19" s="51" t="s">
+      <c r="C19" s="37"/>
+      <c r="E19" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="F19" s="50"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="2:6" ht="31.2">
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="E20" s="51" t="s">
+      <c r="C20" s="37"/>
+      <c r="E20" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="F20" s="50"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="2:6" ht="31.2">
-      <c r="B21" s="49" t="s">
+      <c r="B21" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="E21" s="51" t="s">
+      <c r="C21" s="37"/>
+      <c r="E21" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="F21" s="50"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="50"/>
-      <c r="E22" s="51" t="s">
+      <c r="C22" s="37"/>
+      <c r="E22" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="F22" s="50"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="49" t="s">
+      <c r="B23" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="E23" s="51" t="s">
+      <c r="C23" s="37"/>
+      <c r="E23" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="F23" s="50"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="2:6">
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="E24" s="51" t="s">
+      <c r="C24" s="37"/>
+      <c r="E24" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="50"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="E25" s="54" t="s">
+      <c r="C25" s="40"/>
+      <c r="E25" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="F25" s="53"/>
+      <c r="F25" s="40"/>
     </row>
     <row r="27" spans="2:6" ht="16.95" customHeight="1">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="E27" s="7" t="s">
+      <c r="C27" s="69"/>
+      <c r="E27" s="70" t="s">
         <v>176</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="70"/>
     </row>
     <row r="28" spans="2:6" ht="31.2">
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="E28" s="51" t="s">
+      <c r="C28" s="37"/>
+      <c r="E28" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="F28" s="50"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="E29" s="51" t="s">
+      <c r="C29" s="37"/>
+      <c r="E29" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="50"/>
+      <c r="F29" s="37"/>
     </row>
     <row r="30" spans="2:6" ht="31.2">
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="E30" s="51" t="s">
+      <c r="C30" s="37"/>
+      <c r="E30" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="F30" s="50"/>
+      <c r="F30" s="37"/>
     </row>
     <row r="31" spans="2:6" ht="33" customHeight="1">
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="E31" s="51" t="s">
+      <c r="C31" s="37"/>
+      <c r="E31" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="F31" s="50"/>
+      <c r="F31" s="37"/>
     </row>
     <row r="32" spans="2:6" ht="31.2">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="E32" s="51" t="s">
+      <c r="C32" s="37"/>
+      <c r="E32" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="37"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="E33" s="51" t="s">
+      <c r="C33" s="37"/>
+      <c r="E33" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="37"/>
     </row>
     <row r="34" spans="2:7" ht="31.2">
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="E34" s="54" t="s">
+      <c r="C34" s="37"/>
+      <c r="E34" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="F34" s="53"/>
+      <c r="F34" s="40"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="C35" s="50"/>
+      <c r="C35" s="37"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="C36" s="50"/>
+      <c r="C36" s="37"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="C37" s="53"/>
+      <c r="C37" s="40"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="31" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3652,32 +3671,32 @@
       </c>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="55"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="55"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="46">
+      <c r="A50" s="33">
         <v>1</v>
       </c>
       <c r="B50" t="s">
@@ -3685,7 +3704,7 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="46">
+      <c r="A51" s="33">
         <v>2</v>
       </c>
       <c r="B51" t="s">
@@ -3693,7 +3712,7 @@
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="46">
+      <c r="A52" s="33">
         <v>3</v>
       </c>
       <c r="B52" t="s">
@@ -3701,7 +3720,7 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="46">
+      <c r="A53" s="33">
         <v>4</v>
       </c>
       <c r="B53" t="s">
@@ -3709,7 +3728,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="46">
+      <c r="A54" s="33">
         <v>5</v>
       </c>
       <c r="B54" t="s">
@@ -3717,7 +3736,7 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="24" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3737,25 +3756,25 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="90" customHeight="1">
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="67" t="s">
         <v>198</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="67"/>
+      <c r="F63" s="67"/>
     </row>
     <row r="66" spans="1:6" ht="84" customHeight="1">
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="67"/>
+      <c r="F66" s="67"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="24" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3765,7 +3784,7 @@
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="46">
+      <c r="A71" s="33">
         <v>1</v>
       </c>
       <c r="B71" t="s">
@@ -3776,7 +3795,7 @@
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="46">
+      <c r="A72" s="33">
         <v>2</v>
       </c>
       <c r="B72" t="s">
@@ -3787,7 +3806,7 @@
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="46">
+      <c r="A73" s="33">
         <v>3</v>
       </c>
       <c r="B73" t="s">
@@ -3798,7 +3817,7 @@
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="46">
+      <c r="A74" s="33">
         <v>4</v>
       </c>
       <c r="B74" t="s">
@@ -3809,69 +3828,69 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="16.05" customHeight="1">
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="68" t="s">
         <v>209</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="68"/>
       <c r="E75" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="B76" s="68"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="68"/>
     </row>
     <row r="77" spans="1:6">
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="B77" s="68"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="68"/>
     </row>
     <row r="78" spans="1:6">
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
+      <c r="B78" s="68"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="68"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
+      <c r="B79" s="68"/>
+      <c r="C79" s="68"/>
+      <c r="D79" s="68"/>
     </row>
     <row r="80" spans="1:6">
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
+      <c r="B80" s="68"/>
+      <c r="C80" s="68"/>
+      <c r="D80" s="68"/>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="B81" s="68"/>
+      <c r="C81" s="68"/>
+      <c r="D81" s="68"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="B82" s="68"/>
+      <c r="C82" s="68"/>
+      <c r="D82" s="68"/>
     </row>
     <row r="83" spans="2:5">
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+      <c r="B83" s="68"/>
+      <c r="C83" s="68"/>
+      <c r="D83" s="68"/>
     </row>
     <row r="84" spans="2:5">
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
+      <c r="B84" s="68"/>
+      <c r="C84" s="68"/>
+      <c r="D84" s="68"/>
     </row>
     <row r="85" spans="2:5">
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="B85" s="68"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="68"/>
     </row>
     <row r="86" spans="2:5">
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
+      <c r="B86" s="68"/>
+      <c r="C86" s="68"/>
+      <c r="D86" s="68"/>
     </row>
     <row r="88" spans="2:5">
       <c r="B88" t="s">
@@ -3884,17 +3903,17 @@
       </c>
     </row>
     <row r="92" spans="2:5">
-      <c r="B92" s="36" t="s">
+      <c r="B92" s="24" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="93" spans="2:5" ht="55.95" customHeight="1">
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="C93" s="67"/>
+      <c r="D93" s="67"/>
+      <c r="E93" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3916,14 +3935,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C27" zoomScale="120" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="5.796875" customWidth="1"/>
-    <col min="2" max="2" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="69.796875" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="49.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.19921875" bestFit="1" customWidth="1"/>
@@ -3936,7 +3955,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="46">
+      <c r="A3" s="33">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -3944,7 +3963,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="46">
+      <c r="A4" s="33">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -3954,11 +3973,11 @@
         <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="46">
+      <c r="A5" s="33">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -3968,14 +3987,14 @@
         <v>216</v>
       </c>
       <c r="D5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="46">
+      <c r="A6" s="33">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -3986,31 +4005,40 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="46">
+      <c r="A7" s="33">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="76" t="s">
         <v>194</v>
       </c>
+      <c r="C7" s="76" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="46">
+      <c r="A8" s="33">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="76" t="s">
         <v>31</v>
       </c>
+      <c r="C8" s="76" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="46">
+      <c r="A9" s="33">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="76" t="s">
         <v>32</v>
       </c>
+      <c r="C9" s="76" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="46">
+      <c r="A10" s="33">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -4021,7 +4049,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="46">
+      <c r="A11" s="33">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -4032,7 +4060,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="46">
+      <c r="A12" s="33">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -4043,7 +4071,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="46">
+      <c r="A13" s="33">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -4051,7 +4079,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="46">
+      <c r="A14" s="33">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -4059,10 +4087,10 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="46">
+      <c r="A15" s="33">
         <v>13</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="25" t="s">
         <v>219</v>
       </c>
       <c r="C15" t="s">
@@ -4070,186 +4098,181 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="46">
+      <c r="A16" s="33">
         <v>14</v>
       </c>
-      <c r="B16" s="37"/>
+      <c r="B16" s="25"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="37"/>
+      <c r="B17" s="25"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="37"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" t="s">
+      <c r="B18" s="25"/>
+    </row>
+    <row r="19" spans="2:6" ht="62.4">
+      <c r="B19" s="55" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="C23" s="71" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" t="s">
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="C24" s="36" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="C24" s="49" t="s">
+      <c r="E24" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="F24" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="E24" s="56" t="s">
+    </row>
+    <row r="25" spans="2:6">
+      <c r="C25" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="F24" s="50" t="s">
+      <c r="D25" s="43" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="C25" s="49" t="s">
+      <c r="E25" s="43">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="D25" s="56" t="s">
-        <v>229</v>
-      </c>
-      <c r="E25" s="56">
-        <v>1000</v>
-      </c>
-      <c r="F25" s="50" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="26" spans="2:6">
-      <c r="C26" s="49"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="50"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="2:6">
-      <c r="C27" s="49"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="50"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="2:6">
-      <c r="C28" s="52"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="53"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="40"/>
     </row>
     <row r="30" spans="2:6">
       <c r="C30" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="C32" s="71" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="C33" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="E33" s="43"/>
+      <c r="F33" s="37"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="C34" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D34" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="E34" s="43"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="C35" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" s="43">
+        <v>1000</v>
+      </c>
+      <c r="E35" s="43"/>
+      <c r="F35" s="37"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="C36" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="E36" s="43"/>
+      <c r="F36" s="37"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="C37" s="45" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="C32" s="4" t="s">
+      <c r="D37" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="C33" s="49" t="s">
-        <v>224</v>
-      </c>
-      <c r="D33" s="56" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="50"/>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="C34" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="D34" s="56" t="s">
-        <v>229</v>
-      </c>
-      <c r="E34" s="56"/>
-      <c r="F34" s="50"/>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="C35" s="49" t="s">
-        <v>226</v>
-      </c>
-      <c r="D35" s="56">
-        <v>1000</v>
-      </c>
-      <c r="E35" s="56"/>
-      <c r="F35" s="50"/>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="C36" s="49" t="s">
-        <v>227</v>
-      </c>
-      <c r="D36" s="56" t="s">
-        <v>230</v>
-      </c>
-      <c r="E36" s="56"/>
-      <c r="F36" s="50"/>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="C37" s="58" t="s">
+      <c r="E37" s="43"/>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="C38" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="D37" s="59" t="s">
+      <c r="D38" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="E37" s="56"/>
-      <c r="F37" s="50"/>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="C38" s="58" t="s">
+      <c r="E38" s="43"/>
+      <c r="F38" s="37"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="C39" s="36"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="37"/>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="C40" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="40" t="s">
         <v>235</v>
-      </c>
-      <c r="D38" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="E38" s="56"/>
-      <c r="F38" s="50"/>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="C39" s="49"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="50"/>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="C40" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="53" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="42" spans="2:6">
       <c r="C42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C52" s="47" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3">
-      <c r="B52" s="36" t="s">
-        <v>240</v>
-      </c>
-      <c r="C52" s="60" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4258,8 +4281,8 @@
     <mergeCell ref="C32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4267,7 +4290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="147" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -4284,39 +4307,39 @@
   <sheetData>
     <row r="2" spans="1:12">
       <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="24" t="s">
         <v>242</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="B3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" t="s">
         <v>245</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>246</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>247</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>241</v>
+      </c>
+      <c r="J3" t="s">
         <v>248</v>
       </c>
-      <c r="F3" t="s">
+      <c r="L3" t="s">
         <v>249</v>
-      </c>
-      <c r="G3" t="s">
-        <v>243</v>
-      </c>
-      <c r="J3" t="s">
-        <v>250</v>
-      </c>
-      <c r="L3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4324,10 +4347,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -4335,10 +4358,10 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -4346,7 +4369,7 @@
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4355,178 +4378,178 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="J8" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="L8" s="36" t="s">
-        <v>257</v>
+      <c r="J8" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="J9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="J10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="J11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="J12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="J13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="J16" s="36" t="s">
-        <v>249</v>
+      <c r="J16" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="J17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="J18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="J19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="J20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="J21" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="J22" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="2:10">
       <c r="J23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="16.05" customHeight="1">
+      <c r="B25" s="72" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="36" t="s">
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+    </row>
+    <row r="26" spans="2:10" ht="34.950000000000003" customHeight="1">
+      <c r="B26" s="72" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" ht="16.05" customHeight="1">
-      <c r="B25" s="3" t="s">
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+    </row>
+    <row r="27" spans="2:10" ht="30" customHeight="1">
+      <c r="B27" s="72" t="s">
         <v>273</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="2:10" ht="34.950000000000003" customHeight="1">
-      <c r="B26" s="3" t="s">
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+    </row>
+    <row r="28" spans="2:10" ht="16.05" customHeight="1">
+      <c r="B28" s="72" t="s">
         <v>274</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="2:10" ht="30" customHeight="1">
-      <c r="B27" s="3" t="s">
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+    </row>
+    <row r="29" spans="2:10" ht="36" customHeight="1">
+      <c r="B29" s="72" t="s">
         <v>275</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="2:10" ht="16.05" customHeight="1">
-      <c r="B28" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="2:10" ht="36" customHeight="1">
-      <c r="B29" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="61"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="61"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="61"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="61"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="61"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="61"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="61"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="61"/>
+      <c r="A38" s="48"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4545,363 +4568,363 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.69921875" style="62" customWidth="1"/>
-    <col min="2" max="2" width="10.296875" style="62" customWidth="1"/>
-    <col min="3" max="3" width="29" style="62" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" style="63" customWidth="1"/>
-    <col min="5" max="5" width="29.69921875" style="62" customWidth="1"/>
-    <col min="6" max="6" width="10.796875" style="62"/>
-    <col min="7" max="7" width="17" style="62" customWidth="1"/>
-    <col min="8" max="8" width="12.19921875" style="62" customWidth="1"/>
-    <col min="9" max="9" width="45.69921875" style="64" customWidth="1"/>
-    <col min="10" max="1024" width="10.796875" style="62"/>
+    <col min="1" max="1" width="3.69921875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="10.296875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="29" style="49" customWidth="1"/>
+    <col min="4" max="4" width="12.19921875" style="50" customWidth="1"/>
+    <col min="5" max="5" width="29.69921875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" style="49"/>
+    <col min="7" max="7" width="17" style="49" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" style="49" customWidth="1"/>
+    <col min="9" max="9" width="45.69921875" style="51" customWidth="1"/>
+    <col min="10" max="1024" width="10.796875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="65" customFormat="1">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" s="52" customFormat="1">
+      <c r="B1" s="74" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="74"/>
+      <c r="D1" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" s="54"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="49" t="s">
         <v>278</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="66" t="s">
+      <c r="B2" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="67"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="62" t="s">
+      <c r="C2" s="73"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="50">
+        <v>3</v>
+      </c>
+      <c r="H3" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="I3" s="55"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="50">
+        <v>5</v>
+      </c>
+      <c r="G4" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="C3" s="62" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="63">
+      <c r="H4" s="56" t="s">
+        <v>282</v>
+      </c>
+      <c r="I4" s="55" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="50">
+        <v>10</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>284</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="31.2">
+      <c r="C6" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="50">
+        <v>15</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="49" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>291</v>
+      </c>
+      <c r="C7" s="73"/>
+      <c r="G7" s="49" t="s">
+        <v>292</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>293</v>
+      </c>
+      <c r="I7" s="55" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="50">
+        <v>15</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>295</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>296</v>
+      </c>
+      <c r="I8" s="55" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="C10" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="C11" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="50">
         <v>3</v>
       </c>
-      <c r="H3" s="62" t="s">
-        <v>282</v>
-      </c>
-      <c r="I3" s="68"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="C4" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="63">
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="49" t="s">
+        <v>298</v>
+      </c>
+      <c r="B12" s="73" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" s="73"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="42">
         <v>5</v>
       </c>
-      <c r="G4" s="62" t="s">
-        <v>283</v>
-      </c>
-      <c r="H4" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="I4" s="68" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="C5" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="63">
+    </row>
+    <row r="15" spans="1:9">
+      <c r="C15" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="42">
         <v>10</v>
       </c>
-      <c r="G5" s="62" t="s">
-        <v>286</v>
-      </c>
-      <c r="H5" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="I5" s="68" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="31.2">
-      <c r="C6" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="63">
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="42">
         <v>15</v>
       </c>
-      <c r="G6" s="62" t="s">
-        <v>289</v>
-      </c>
-      <c r="H6" s="71" t="s">
-        <v>290</v>
-      </c>
-      <c r="I6" s="68" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="62" t="s">
-        <v>292</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="G7" s="62" t="s">
-        <v>294</v>
-      </c>
-      <c r="H7" s="72" t="s">
-        <v>295</v>
-      </c>
-      <c r="I7" s="68" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="C8" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="63">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="49" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="73"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="C20" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="50">
         <v>15</v>
       </c>
-      <c r="G8" s="62" t="s">
-        <v>297</v>
-      </c>
-      <c r="H8" s="73" t="s">
-        <v>298</v>
-      </c>
-      <c r="I8" s="68" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="63">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" s="73" t="s">
+        <v>303</v>
+      </c>
+      <c r="C21" s="73"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="C23" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="C24" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="50">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="C10" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="63">
+    <row r="25" spans="1:5">
+      <c r="A25" s="49" t="s">
+        <v>304</v>
+      </c>
+      <c r="B25" s="73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="73"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="50">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="C11" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="63">
+    <row r="27" spans="1:5">
+      <c r="B27" s="61"/>
+      <c r="C27" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="C28" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="31.2">
+      <c r="A29" s="49" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>306</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" s="62" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="C31" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="C32" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="C33" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="50">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="62" t="s">
-        <v>300</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="55">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="C14" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="55">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="C15" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="55">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="C16" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="55">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="62" t="s">
-        <v>302</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="C18" s="62" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="C19" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="C20" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="63">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="62" t="s">
-        <v>304</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="C22" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="C23" s="62" t="s">
-        <v>120</v>
-      </c>
-      <c r="D23" s="63">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="C24" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="62" t="s">
-        <v>306</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="36" spans="2:4">
+      <c r="B36" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="C26" s="62" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="74"/>
-      <c r="C27" s="62" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" s="63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="C28" s="62" t="s">
-        <v>125</v>
-      </c>
-      <c r="D28" s="63">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="31.2">
-      <c r="A29" s="62" t="s">
-        <v>307</v>
-      </c>
-      <c r="B29" s="62" t="s">
-        <v>308</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29" s="75" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="C30" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="63">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="C31" s="62" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="C32" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" s="63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="C33" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="63">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" s="62" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="62" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="49" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>